<commit_message>
add IMortality to speadsheet
</commit_message>
<xml_diff>
--- a/Team_Shuhart_Smith/Shuhart_Smith_Ecosystem_OOP/OOP_Map.xlsx
+++ b/Team_Shuhart_Smith/Shuhart_Smith_Ecosystem_OOP/OOP_Map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Ecosystem</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Interfaces</t>
+  </si>
+  <si>
+    <t>interface Imortality</t>
   </si>
 </sst>
 </file>
@@ -574,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,12 +924,10 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>31</v>
-      </c>
+      <c r="F22" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
@@ -941,7 +942,7 @@
         <v>28</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -957,7 +958,7 @@
         <v>28</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
@@ -970,10 +971,10 @@
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
@@ -989,17 +990,33 @@
         <v>29</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
       <c r="F27" s="17" t="s">
         <v>29</v>
       </c>
       <c r="G27" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F28" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" s="15" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add probability of interfaces to Lion and Trees, and other commentary
</commit_message>
<xml_diff>
--- a/Team_Shuhart_Smith/Shuhart_Smith_Ecosystem_OOP/OOP_Map.xlsx
+++ b/Team_Shuhart_Smith/Shuhart_Smith_Ecosystem_OOP/OOP_Map.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>Ecosystem</t>
   </si>
@@ -141,6 +141,18 @@
   </si>
   <si>
     <t>interface Imortality</t>
+  </si>
+  <si>
+    <t>implements  IGivesBirth</t>
+  </si>
+  <si>
+    <t>implements  IMortal</t>
+  </si>
+  <si>
+    <t>Park extends Habitat</t>
+  </si>
+  <si>
+    <t>Lake extends Habitat</t>
   </si>
 </sst>
 </file>
@@ -196,7 +208,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -247,25 +259,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -275,28 +330,58 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,441 +680,469 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="12" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="12" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="11" t="s">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="12" t="s">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="10" t="s">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="12" t="s">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="12" t="s">
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F11" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="12" t="s">
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F12" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="14" t="s">
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="12" t="s">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2" t="s">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="18" t="s">
+      <c r="A18" s="12"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="15" t="s">
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="15" t="s">
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="15" t="s">
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="15" t="s">
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="17" t="s">
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G25" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24" s="15" t="s">
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" s="15" t="s">
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="17" t="s">
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G28" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G27" s="15" t="s">
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F28" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G28" s="15" t="s">
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F30" s="24"/>
+      <c r="G30" s="7" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="A2:A16"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C5:C12"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="B2:B12"/>
+  <mergeCells count="12">
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="A2:A18"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C7:C14"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="B2:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add offspringSize under each declared animal
</commit_message>
<xml_diff>
--- a/Team_Shuhart_Smith/Shuhart_Smith_Ecosystem_OOP/OOP_Map.xlsx
+++ b/Team_Shuhart_Smith/Shuhart_Smith_Ecosystem_OOP/OOP_Map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>Ecosystem</t>
   </si>
@@ -153,6 +153,42 @@
   </si>
   <si>
     <t>Abstract Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 pup</t>
+  </si>
+  <si>
+    <t>2000 eggs</t>
+  </si>
+  <si>
+    <t>1 million</t>
+  </si>
+  <si>
+    <t>http://www.gma.org/fogm/Gadus_callarias.htm</t>
+  </si>
+  <si>
+    <t>http://www.fcps.edu/islandcreekes/ecology/largemouth_bass.htm</t>
+  </si>
+  <si>
+    <t>http://www.defenders.org/bats/bats</t>
+  </si>
+  <si>
+    <t>https://lionalert.org/page/reproduction-and-offspring</t>
+  </si>
+  <si>
+    <t>3 cubs</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Canine_reproduction</t>
+  </si>
+  <si>
+    <t>http://animals.mom.me/reproduction-cycle-dragonfly-9190.html</t>
+  </si>
+  <si>
+    <t>http://www.terro.com/pantry-moths-reproduction</t>
+  </si>
+  <si>
+    <t>http://www.ehow.com/about_6465166_do-oak-trees-reproduce_.html</t>
   </si>
 </sst>
 </file>
@@ -308,34 +344,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -346,6 +364,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -354,6 +375,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -638,7 +674,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,56 +712,64 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="1"/>
+      <c r="G2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12" t="s">
+      <c r="A3" s="20"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="1"/>
+      <c r="G3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="5"/>
@@ -734,26 +778,30 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="13" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="1"/>
+      <c r="G5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="13" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="9" t="s">
         <v>36</v>
       </c>
       <c r="G6" s="5"/>
@@ -762,113 +810,135 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="16" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="1"/>
+      <c r="G7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="16" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="1"/>
+      <c r="G8" s="5">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11" t="s">
+      <c r="A9" s="21"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="1"/>
+      <c r="G9" s="5">
+        <v>100</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12" t="s">
+      <c r="A10" s="21"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="1"/>
+      <c r="G10" s="5">
+        <v>300</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11" t="s">
+      <c r="A11" s="21"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="1"/>
+      <c r="G11" s="5">
+        <v>10000</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12" t="s">
+      <c r="A12" s="21"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="5"/>
+      <c r="G12" s="5">
+        <v>10000</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11" t="s">
+      <c r="A13" s="21"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="5"/>
@@ -878,11 +948,11 @@
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12" t="s">
+      <c r="A14" s="21"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="8" t="s">
         <v>15</v>
       </c>
       <c r="F14" s="5"/>
@@ -892,11 +962,11 @@
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15" t="s">
+      <c r="A15" s="21"/>
+      <c r="B15" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="5"/>
@@ -908,9 +978,9 @@
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="17" t="s">
+      <c r="A16" s="21"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="11" t="s">
         <v>39</v>
       </c>
       <c r="D16" s="5"/>
@@ -922,9 +992,9 @@
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="17" t="s">
+      <c r="A17" s="21"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="11" t="s">
         <v>40</v>
       </c>
       <c r="D17" s="5"/>
@@ -936,8 +1006,8 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -948,11 +1018,11 @@
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="5"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="13" t="s">
         <v>29</v>
       </c>
       <c r="F19" s="5"/>
@@ -962,11 +1032,11 @@
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="5"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="14" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="5"/>
@@ -980,7 +1050,7 @@
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="5"/>
@@ -994,7 +1064,7 @@
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="14" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="5"/>
@@ -1008,10 +1078,10 @@
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="21" t="s">
+      <c r="E23" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="14" t="s">
         <v>23</v>
       </c>
       <c r="G23" s="1"/>
@@ -1024,8 +1094,8 @@
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="20" t="s">
+      <c r="E24" s="17"/>
+      <c r="F24" s="14" t="s">
         <v>24</v>
       </c>
       <c r="G24" s="1"/>
@@ -1038,8 +1108,8 @@
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="20" t="s">
+      <c r="E25" s="18"/>
+      <c r="F25" s="14" t="s">
         <v>25</v>
       </c>
       <c r="G25" s="1"/>
@@ -1052,10 +1122,10 @@
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="21" t="s">
+      <c r="E26" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F26" s="20" t="s">
+      <c r="F26" s="14" t="s">
         <v>22</v>
       </c>
       <c r="G26" s="1"/>
@@ -1068,8 +1138,8 @@
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="20" t="s">
+      <c r="E27" s="17"/>
+      <c r="F27" s="14" t="s">
         <v>26</v>
       </c>
       <c r="G27" s="1"/>
@@ -1082,8 +1152,8 @@
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="20" t="s">
+      <c r="E28" s="18"/>
+      <c r="F28" s="14" t="s">
         <v>27</v>
       </c>
       <c r="G28" s="1"/>
@@ -1180,11 +1250,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="D4:D8"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="B15:B17"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D13:D14"/>
@@ -1193,6 +1258,11 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="C2:C10"/>
     <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="D4:D8"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="B15:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add arrays for the size and names of spheres
</commit_message>
<xml_diff>
--- a/Team_Shuhart_Smith/Shuhart_Smith_Ecosystem_OOP/OOP_Map.xlsx
+++ b/Team_Shuhart_Smith/Shuhart_Smith_Ecosystem_OOP/OOP_Map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
   <si>
     <t>Ecosystem</t>
   </si>
@@ -155,15 +155,6 @@
     <t>Abstract Class</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1 pup</t>
-  </si>
-  <si>
-    <t>2000 eggs</t>
-  </si>
-  <si>
-    <t>1 million</t>
-  </si>
-  <si>
     <t>http://www.gma.org/fogm/Gadus_callarias.htm</t>
   </si>
   <si>
@@ -176,9 +167,6 @@
     <t>https://lionalert.org/page/reproduction-and-offspring</t>
   </si>
   <si>
-    <t>3 cubs</t>
-  </si>
-  <si>
     <t>https://en.wikipedia.org/wiki/Canine_reproduction</t>
   </si>
   <si>
@@ -189,6 +177,9 @@
   </si>
   <si>
     <t>http://www.ehow.com/about_6465166_do-oak-trees-reproduce_.html</t>
+  </si>
+  <si>
+    <t>Natural Log</t>
   </si>
 </sst>
 </file>
@@ -364,9 +355,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -375,21 +381,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -671,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,9 +676,10 @@
     <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -707,21 +699,24 @@
         <v>17</v>
       </c>
       <c r="G1" s="5"/>
-      <c r="H1" s="1"/>
+      <c r="H1" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="20" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -730,110 +725,128 @@
       <c r="F2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="5">
+        <v>2000</v>
+      </c>
+      <c r="H2" s="5">
+        <f>LN(G2)</f>
+        <v>7.6009024595420822</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="20"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="15"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
       <c r="E3" s="8" t="s">
         <v>31</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="1"/>
+      <c r="G3" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="H3" s="5">
+        <f>LN(G3)</f>
+        <v>13.815510557964274</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="16"/>
       <c r="B4" s="19"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="17" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="5"/>
-      <c r="H4" s="1"/>
+      <c r="H4" s="5"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
       <c r="B5" s="19"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
       <c r="F5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="1"/>
+      <c r="G5" s="5">
+        <v>3</v>
+      </c>
+      <c r="H5" s="5">
+        <f>LN(G5)</f>
+        <v>1.0986122886681098</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="16"/>
       <c r="B6" s="19"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
       <c r="F6" s="9" t="s">
         <v>36</v>
       </c>
       <c r="G6" s="5"/>
-      <c r="H6" s="1"/>
+      <c r="H6" s="5"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="16"/>
       <c r="B7" s="19"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
       <c r="E7" s="10" t="s">
         <v>37</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I7" s="1"/>
+      <c r="G7" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="H7" s="5">
+        <f>LN(G7)</f>
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="16"/>
       <c r="B8" s="19"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
       <c r="E8" s="10" t="s">
         <v>38</v>
       </c>
@@ -843,17 +856,21 @@
       <c r="G8" s="5">
         <v>5</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I8" s="1"/>
+      <c r="H8" s="5">
+        <f>LN(G8)</f>
+        <v>1.6094379124341003</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="16"/>
       <c r="B9" s="19"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15" t="s">
+      <c r="C9" s="17"/>
+      <c r="D9" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="8" t="s">
@@ -865,17 +882,21 @@
       <c r="G9" s="5">
         <v>100</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I9" s="1"/>
+      <c r="H9" s="5">
+        <f>LN(G9)</f>
+        <v>4.6051701859880918</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="16"/>
       <c r="B10" s="19"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="8" t="s">
         <v>33</v>
       </c>
@@ -885,17 +906,21 @@
       <c r="G10" s="5">
         <v>300</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I10" s="1"/>
+      <c r="H10" s="5">
+        <f>LN(G10)</f>
+        <v>5.7037824746562009</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
       <c r="B11" s="19"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15" t="s">
+      <c r="C11" s="17"/>
+      <c r="D11" s="17" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="8" t="s">
@@ -907,17 +932,21 @@
       <c r="G11" s="5">
         <v>10000</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I11" s="1"/>
+      <c r="H11" s="5">
+        <f>LN(G11)</f>
+        <v>9.2103403719761836</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
       <c r="B12" s="19"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
       <c r="E12" s="8" t="s">
         <v>12</v>
       </c>
@@ -927,15 +956,19 @@
       <c r="G12" s="5">
         <v>10000</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="5">
+        <f>LN(G12)</f>
+        <v>9.2103403719761836</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="21"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
       <c r="B13" s="19"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15" t="s">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="8" t="s">
@@ -943,26 +976,28 @@
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="1"/>
+      <c r="H13" s="5"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="21"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="16"/>
       <c r="B14" s="19"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="8" t="s">
         <v>15</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="1"/>
+      <c r="H14" s="5"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
       <c r="B15" s="19" t="s">
         <v>5</v>
       </c>
@@ -973,12 +1008,13 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="1"/>
+      <c r="H15" s="5"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="16"/>
       <c r="B16" s="19"/>
       <c r="C16" s="11" t="s">
         <v>39</v>
@@ -987,12 +1023,13 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="5"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="21"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
       <c r="B17" s="19"/>
       <c r="C17" s="11" t="s">
         <v>40</v>
@@ -1001,11 +1038,12 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="1"/>
+      <c r="H17" s="5"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
       <c r="C18" s="5"/>
@@ -1013,11 +1051,12 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="1"/>
+      <c r="H18" s="5"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="5"/>
@@ -1030,8 +1069,9 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="5"/>
@@ -1044,8 +1084,9 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1058,8 +1099,9 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1072,13 +1114,14 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="21" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="14" t="s">
@@ -1088,13 +1131,14 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="17"/>
+      <c r="E24" s="22"/>
       <c r="F24" s="14" t="s">
         <v>24</v>
       </c>
@@ -1102,13 +1146,14 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="18"/>
+      <c r="E25" s="23"/>
       <c r="F25" s="14" t="s">
         <v>25</v>
       </c>
@@ -1116,13 +1161,14 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="21" t="s">
         <v>41</v>
       </c>
       <c r="F26" s="14" t="s">
@@ -1132,13 +1178,14 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="17"/>
+      <c r="E27" s="22"/>
       <c r="F27" s="14" t="s">
         <v>26</v>
       </c>
@@ -1146,21 +1193,23 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="18"/>
+      <c r="E28" s="23"/>
       <c r="F28" s="14" t="s">
         <v>27</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1170,8 +1219,9 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1181,8 +1231,9 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1192,8 +1243,9 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1203,8 +1255,9 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1214,8 +1267,9 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1225,8 +1279,9 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1236,8 +1291,9 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1247,9 +1303,15 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="D4:D8"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="B15:B17"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D13:D14"/>
@@ -1258,11 +1320,6 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="C2:C10"/>
     <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="D4:D8"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="B15:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>